<commit_message>
some bugs fixed, function rectified.
- Added output to a new, named sheet of outfile.xslx
- Another sheet within outfile.xlsx to have statistics of marks as output
</commit_message>
<xml_diff>
--- a/process-course-marks-r/outfile.xlsx
+++ b/process-course-marks-r/outfile.xlsx
@@ -6,13 +6,13 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="All Marks" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="129">
   <si>
     <t xml:space="preserve">RollNo</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t xml:space="preserve">W.A.Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W.C.Total</t>
   </si>
   <si>
     <t xml:space="preserve">20110209</t>
@@ -443,9 +446,9 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:AI31" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:AI31"/>
-  <tableColumns count="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:AJ31" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:AJ31"/>
+  <tableColumns count="36">
     <tableColumn id="1" name="RollNo"/>
     <tableColumn id="2" name="Student.Name"/>
     <tableColumn id="3" name="Email.Id"/>
@@ -481,6 +484,7 @@
     <tableColumn id="33" name="Norm.Total"/>
     <tableColumn id="34" name="Grade"/>
     <tableColumn id="35" name="W.A.Total"/>
+    <tableColumn id="36" name="W.C.Total"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -877,22 +881,25 @@
       <c r="AI1" t="s">
         <v>34</v>
       </c>
+      <c r="AJ1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -982,24 +989,27 @@
         <v>0</v>
       </c>
       <c r="AI2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
         <v>40</v>
-      </c>
-      <c r="B3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" t="s">
-        <v>39</v>
       </c>
       <c r="F3" t="n">
         <v>82</v>
@@ -1038,7 +1048,7 @@
         <v>0</v>
       </c>
       <c r="R3" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S3" t="n">
         <v>2</v>
@@ -1090,23 +1100,26 @@
       </c>
       <c r="AI3" t="n">
         <v>34.36</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F4" t="n">
         <v>83</v>
@@ -1145,7 +1158,7 @@
         <v>0</v>
       </c>
       <c r="R4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S4" t="n">
         <v>1</v>
@@ -1197,23 +1210,26 @@
       </c>
       <c r="AI4" t="n">
         <v>33.84</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F5" t="n">
         <v>9.2</v>
@@ -1252,7 +1268,7 @@
         <v>0</v>
       </c>
       <c r="R5" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S5" t="n">
         <v>1</v>
@@ -1304,23 +1320,26 @@
       </c>
       <c r="AI5" t="n">
         <v>18.79</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>12.5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F6" t="n">
         <v>68</v>
@@ -1359,7 +1378,7 @@
         <v>0</v>
       </c>
       <c r="R6" t="n">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="S6" t="n">
         <v>0</v>
@@ -1411,23 +1430,26 @@
       </c>
       <c r="AI6" t="n">
         <v>30.67</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>3.75</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -1466,7 +1488,7 @@
         <v>2</v>
       </c>
       <c r="R7" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S7" t="n">
         <v>2</v>
@@ -1518,23 +1540,26 @@
       </c>
       <c r="AI7" t="n">
         <v>15.9</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F8" t="n">
         <v>76.5</v>
@@ -1573,7 +1598,7 @@
         <v>0</v>
       </c>
       <c r="R8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S8" t="n">
         <v>1</v>
@@ -1625,23 +1650,26 @@
       </c>
       <c r="AI8" t="n">
         <v>32.43</v>
+      </c>
+      <c r="AJ8" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F9" t="n">
         <v>48</v>
@@ -1680,7 +1708,7 @@
         <v>0</v>
       </c>
       <c r="R9" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S9" t="n">
         <v>2</v>
@@ -1732,23 +1760,26 @@
       </c>
       <c r="AI9" t="n">
         <v>16.29</v>
+      </c>
+      <c r="AJ9" t="n">
+        <v>1.25</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F10" t="n">
         <v>23</v>
@@ -1787,7 +1818,7 @@
         <v>0</v>
       </c>
       <c r="R10" t="n">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="S10" t="n">
         <v>1</v>
@@ -1839,23 +1870,26 @@
       </c>
       <c r="AI10" t="n">
         <v>5.57</v>
+      </c>
+      <c r="AJ10" t="n">
+        <v>6.25</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F11" t="n">
         <v>80</v>
@@ -1894,7 +1928,7 @@
         <v>0</v>
       </c>
       <c r="R11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S11" t="n">
         <v>1</v>
@@ -1946,23 +1980,26 @@
       </c>
       <c r="AI11" t="n">
         <v>33.57</v>
+      </c>
+      <c r="AJ11" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F12" t="n">
         <v>48.43</v>
@@ -2001,7 +2038,7 @@
         <v>2</v>
       </c>
       <c r="R12" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S12" t="n">
         <v>2</v>
@@ -2053,23 +2090,26 @@
       </c>
       <c r="AI12" t="n">
         <v>27.93</v>
+      </c>
+      <c r="AJ12" t="n">
+        <v>12.5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C13" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F13" t="n">
         <v>73</v>
@@ -2108,7 +2148,7 @@
         <v>2</v>
       </c>
       <c r="R13" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S13" t="n">
         <v>1</v>
@@ -2160,23 +2200,26 @@
       </c>
       <c r="AI13" t="n">
         <v>23.66</v>
+      </c>
+      <c r="AJ13" t="n">
+        <v>12.5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C14" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F14" t="n">
         <v>78</v>
@@ -2215,7 +2258,7 @@
         <v>0</v>
       </c>
       <c r="R14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S14" t="n">
         <v>2</v>
@@ -2267,23 +2310,26 @@
       </c>
       <c r="AI14" t="n">
         <v>27.27</v>
+      </c>
+      <c r="AJ14" t="n">
+        <v>2.5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B15" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C15" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -2322,7 +2368,7 @@
         <v>0</v>
       </c>
       <c r="R15" t="n">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="S15" t="n">
         <v>2</v>
@@ -2374,23 +2420,26 @@
       </c>
       <c r="AI15" t="n">
         <v>9.18</v>
+      </c>
+      <c r="AJ15" t="n">
+        <v>8.75</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B16" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C16" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F16" t="n">
         <v>56</v>
@@ -2429,7 +2478,7 @@
         <v>0</v>
       </c>
       <c r="R16" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="S16" t="n">
         <v>1</v>
@@ -2481,23 +2530,26 @@
       </c>
       <c r="AI16" t="n">
         <v>28.68</v>
+      </c>
+      <c r="AJ16" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B17" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C17" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F17" t="n">
         <v>21.34</v>
@@ -2536,7 +2588,7 @@
         <v>2</v>
       </c>
       <c r="R17" t="n">
-        <v>0</v>
+        <v>4.25</v>
       </c>
       <c r="S17" t="n">
         <v>1</v>
@@ -2588,23 +2640,26 @@
       </c>
       <c r="AI17" t="n">
         <v>11.39</v>
+      </c>
+      <c r="AJ17" t="n">
+        <v>10.62</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B18" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C18" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F18" t="n">
         <v>40</v>
@@ -2643,7 +2698,7 @@
         <v>0</v>
       </c>
       <c r="R18" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S18" t="n">
         <v>1</v>
@@ -2695,23 +2750,26 @@
       </c>
       <c r="AI18" t="n">
         <v>15.24</v>
+      </c>
+      <c r="AJ18" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B19" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C19" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E19" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F19" t="n">
         <v>76</v>
@@ -2750,7 +2808,7 @@
         <v>2</v>
       </c>
       <c r="R19" t="n">
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="S19" t="n">
         <v>1</v>
@@ -2802,23 +2860,26 @@
       </c>
       <c r="AI19" t="n">
         <v>24.89</v>
+      </c>
+      <c r="AJ19" t="n">
+        <v>18.75</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B20" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C20" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F20" t="n">
         <v>58.5</v>
@@ -2857,7 +2918,7 @@
         <v>2</v>
       </c>
       <c r="R20" t="n">
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="S20" t="n">
         <v>2</v>
@@ -2909,23 +2970,26 @@
       </c>
       <c r="AI20" t="n">
         <v>29.93</v>
+      </c>
+      <c r="AJ20" t="n">
+        <v>13.75</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B21" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C21" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E21" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F21" t="n">
         <v>44</v>
@@ -2964,7 +3028,7 @@
         <v>0</v>
       </c>
       <c r="R21" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S21" t="n">
         <v>1</v>
@@ -3016,23 +3080,26 @@
       </c>
       <c r="AI21" t="n">
         <v>21.2</v>
+      </c>
+      <c r="AJ21" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B22" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C22" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E22" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F22" t="n">
         <v>52</v>
@@ -3071,7 +3138,7 @@
         <v>0</v>
       </c>
       <c r="R22" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S22" t="n">
         <v>2</v>
@@ -3123,23 +3190,26 @@
       </c>
       <c r="AI22" t="n">
         <v>18.11</v>
+      </c>
+      <c r="AJ22" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B23" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C23" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E23" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F23" t="n">
         <v>50</v>
@@ -3178,7 +3248,7 @@
         <v>0</v>
       </c>
       <c r="R23" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S23" t="n">
         <v>1</v>
@@ -3230,23 +3300,26 @@
       </c>
       <c r="AI23" t="n">
         <v>9.99</v>
+      </c>
+      <c r="AJ23" t="n">
+        <v>7.5</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B24" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C24" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E24" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F24" t="n">
         <v>65</v>
@@ -3285,7 +3358,7 @@
         <v>0</v>
       </c>
       <c r="R24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S24" t="n">
         <v>2</v>
@@ -3337,23 +3410,26 @@
       </c>
       <c r="AI24" t="n">
         <v>23.44</v>
+      </c>
+      <c r="AJ24" t="n">
+        <v>2.5</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B25" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C25" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E25" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F25" t="n">
         <v>0</v>
@@ -3392,7 +3468,7 @@
         <v>2</v>
       </c>
       <c r="R25" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S25" t="n">
         <v>2</v>
@@ -3444,23 +3520,26 @@
       </c>
       <c r="AI25" t="n">
         <v>25.59</v>
+      </c>
+      <c r="AJ25" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B26" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C26" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E26" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F26" t="n">
         <v>0</v>
@@ -3550,24 +3629,27 @@
         <v>0</v>
       </c>
       <c r="AI26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ26" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B27" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C27" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D27" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F27" t="n">
         <v>0</v>
@@ -3606,7 +3688,7 @@
         <v>2</v>
       </c>
       <c r="R27" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S27" t="n">
         <v>2</v>
@@ -3658,23 +3740,26 @@
       </c>
       <c r="AI27" t="n">
         <v>13.63</v>
+      </c>
+      <c r="AJ27" t="n">
+        <v>7.5</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B28" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C28" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F28" t="n">
         <v>14.9986065954482</v>
@@ -3713,7 +3798,7 @@
         <v>2</v>
       </c>
       <c r="R28" t="n">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="S28" t="n">
         <v>2</v>
@@ -3765,23 +3850,26 @@
       </c>
       <c r="AI28" t="n">
         <v>25.92</v>
+      </c>
+      <c r="AJ28" t="n">
+        <v>11.25</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B29" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C29" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D29" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E29" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F29" t="n">
         <v>86</v>
@@ -3820,7 +3908,7 @@
         <v>2</v>
       </c>
       <c r="R29" t="n">
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="S29" t="n">
         <v>2</v>
@@ -3872,23 +3960,26 @@
       </c>
       <c r="AI29" t="n">
         <v>23.98</v>
+      </c>
+      <c r="AJ29" t="n">
+        <v>13.75</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
+        <v>124</v>
+      </c>
+      <c r="B30" t="s">
+        <v>125</v>
+      </c>
+      <c r="C30" t="s">
+        <v>126</v>
+      </c>
+      <c r="D30" t="s">
         <v>123</v>
       </c>
-      <c r="B30" t="s">
-        <v>124</v>
-      </c>
-      <c r="C30" t="s">
-        <v>125</v>
-      </c>
-      <c r="D30" t="s">
-        <v>122</v>
-      </c>
       <c r="E30" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F30" t="n">
         <v>87</v>
@@ -3927,7 +4018,7 @@
         <v>2</v>
       </c>
       <c r="R30" t="n">
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="S30" t="n">
         <v>2</v>
@@ -3979,23 +4070,26 @@
       </c>
       <c r="AI30" t="n">
         <v>34.28</v>
+      </c>
+      <c r="AJ30" t="n">
+        <v>16.25</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B31" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C31" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D31" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E31" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F31" t="n">
         <v>100</v>
@@ -4034,7 +4128,7 @@
         <v>2</v>
       </c>
       <c r="R31" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="S31" t="n">
         <v>2</v>
@@ -4086,6 +4180,9 @@
       </c>
       <c r="AI31" t="n">
         <v>40</v>
+      </c>
+      <c r="AJ31" t="n">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>